<commit_message>
Fix of the issue  -  Purchase quantity is accepted as zero
</commit_message>
<xml_diff>
--- a/Library_Stock/Sales_Statement/template/stock_sales_account_template.xlsx
+++ b/Library_Stock/Sales_Statement/template/stock_sales_account_template.xlsx
@@ -946,7 +946,7 @@
       </c>
       <c r="F3" s="13" t="inlineStr">
         <is>
-          <t>06-Jun-2021</t>
+          <t>05-Jul-2021</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="F8" s="15" t="inlineStr">
         <is>
-          <t>238.0</t>
+          <t>1209.0</t>
         </is>
       </c>
       <c r="G8" s="10" t="n"/>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="F9" s="22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       <c r="F16" s="24" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="23" t="inlineStr"/>
+      <c r="A17" s="40" t="inlineStr"/>
       <c r="B17" s="23" t="inlineStr"/>
       <c r="C17" s="23" t="inlineStr"/>
       <c r="D17" s="24" t="inlineStr"/>
@@ -1150,52 +1150,52 @@
       <c r="F17" s="24" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="23" t="n"/>
-      <c r="B18" s="23" t="n"/>
-      <c r="C18" s="23" t="n"/>
-      <c r="D18" s="24" t="n"/>
-      <c r="E18" s="24" t="n"/>
-      <c r="F18" s="24" t="n"/>
+      <c r="A18" s="40" t="inlineStr"/>
+      <c r="B18" s="23" t="inlineStr"/>
+      <c r="C18" s="23" t="inlineStr"/>
+      <c r="D18" s="24" t="inlineStr"/>
+      <c r="E18" s="24" t="inlineStr"/>
+      <c r="F18" s="24" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="23" t="n"/>
-      <c r="B19" s="23" t="n"/>
-      <c r="C19" s="23" t="n"/>
-      <c r="D19" s="24" t="n"/>
-      <c r="E19" s="24" t="n"/>
-      <c r="F19" s="24" t="n"/>
+      <c r="A19" s="40" t="inlineStr"/>
+      <c r="B19" s="23" t="inlineStr"/>
+      <c r="C19" s="23" t="inlineStr"/>
+      <c r="D19" s="24" t="inlineStr"/>
+      <c r="E19" s="24" t="inlineStr"/>
+      <c r="F19" s="24" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="23" t="n"/>
-      <c r="B20" s="23" t="n"/>
-      <c r="C20" s="23" t="n"/>
-      <c r="D20" s="24" t="n"/>
-      <c r="E20" s="24" t="n"/>
-      <c r="F20" s="24" t="n"/>
+      <c r="A20" s="40" t="inlineStr"/>
+      <c r="B20" s="23" t="inlineStr"/>
+      <c r="C20" s="23" t="inlineStr"/>
+      <c r="D20" s="24" t="inlineStr"/>
+      <c r="E20" s="24" t="inlineStr"/>
+      <c r="F20" s="24" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="23" t="n"/>
-      <c r="B21" s="23" t="n"/>
-      <c r="C21" s="23" t="n"/>
-      <c r="D21" s="24" t="n"/>
-      <c r="E21" s="24" t="n"/>
-      <c r="F21" s="24" t="n"/>
+      <c r="A21" s="40" t="inlineStr"/>
+      <c r="B21" s="23" t="inlineStr"/>
+      <c r="C21" s="23" t="inlineStr"/>
+      <c r="D21" s="24" t="inlineStr"/>
+      <c r="E21" s="24" t="inlineStr"/>
+      <c r="F21" s="24" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="23" t="n"/>
-      <c r="B22" s="23" t="n"/>
-      <c r="C22" s="23" t="n"/>
-      <c r="D22" s="24" t="n"/>
-      <c r="E22" s="24" t="n"/>
-      <c r="F22" s="24" t="n"/>
+      <c r="A22" s="40" t="inlineStr"/>
+      <c r="B22" s="23" t="inlineStr"/>
+      <c r="C22" s="23" t="inlineStr"/>
+      <c r="D22" s="24" t="inlineStr"/>
+      <c r="E22" s="24" t="inlineStr"/>
+      <c r="F22" s="24" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="23" t="n"/>
-      <c r="B23" s="23" t="n"/>
-      <c r="C23" s="23" t="n"/>
-      <c r="D23" s="24" t="n"/>
-      <c r="E23" s="24" t="n"/>
-      <c r="F23" s="24" t="n"/>
+      <c r="A23" s="23" t="inlineStr"/>
+      <c r="B23" s="23" t="inlineStr"/>
+      <c r="C23" s="23" t="inlineStr"/>
+      <c r="D23" s="24" t="inlineStr"/>
+      <c r="E23" s="24" t="inlineStr"/>
+      <c r="F23" s="24" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="23" t="n"/>

</xml_diff>